<commit_message>
Add one more user
</commit_message>
<xml_diff>
--- a/MathPractiseApplication/Data/Users.xlsx
+++ b/MathPractiseApplication/Data/Users.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Id</t>
   </si>
@@ -23,10 +23,25 @@
     <t>Password</t>
   </si>
   <si>
+    <t>CompletedExercises</t>
+  </si>
+  <si>
+    <t>TestResults</t>
+  </si>
+  <si>
+    <t>Dima1</t>
+  </si>
+  <si>
+    <t>123321</t>
+  </si>
+  <si>
+    <t>4/20</t>
+  </si>
+  <si>
     <t>Dima</t>
   </si>
   <si>
-    <t>123321</t>
+    <t>3/20</t>
   </si>
 </sst>
 </file>
@@ -72,7 +87,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -88,16 +103,45 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="D2" s="0">
+        <v>0</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="0">
+        <v>1</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>